<commit_message>
finish debug, ready to verity correctness
</commit_message>
<xml_diff>
--- a/data/A/input_vehicle_type.xlsx
+++ b/data/A/input_vehicle_type.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView windowWidth="20385" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Vehicle_data" sheetId="1" r:id="rId1"/>
     <sheet name="Description" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
   <si>
     <t xml:space="preserve">vehicle_type_ID      </t>
   </si>
@@ -48,7 +48,6 @@
   </si>
   <si>
     <t>unlimited</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>TRUCK</t>
@@ -99,26 +98,31 @@
     <t>持续里程(m)</t>
   </si>
   <si>
+    <t>充电时间(h)</t>
+  </si>
+  <si>
     <t>每公里运输成本(元)</t>
   </si>
   <si>
     <t>车辆使用成本(元/天)</t>
-  </si>
-  <si>
-    <t>充电时间(h)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -126,32 +130,167 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,8 +303,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -175,107 +500,393 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -324,7 +935,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -359,7 +970,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -562,285 +1173,284 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="15.8833333333333" style="7" customWidth="1"/>
+    <col min="2" max="2" width="17" style="7" customWidth="1"/>
+    <col min="3" max="3" width="13.4416666666667" style="7" customWidth="1"/>
+    <col min="4" max="4" width="12.8833333333333" style="7" customWidth="1"/>
+    <col min="5" max="5" width="10.775" style="7" customWidth="1"/>
+    <col min="6" max="6" width="14.4416666666667" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.8833333333333" style="7" customWidth="1"/>
+    <col min="8" max="8" width="13.5583333333333" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="8.88333333333333" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="15" spans="1:9">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+    <row r="2" ht="15" spans="1:9">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="11">
         <v>12</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="11">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="11">
         <v>100000</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="11">
         <v>0.5</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="11">
         <v>12</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="11">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+    <row r="3" ht="15" spans="1:9">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="11">
         <v>16</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="11">
         <v>2.5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="11">
         <v>120000</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="11">
         <v>0.5</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="11">
         <v>14</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="11">
         <v>300</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="18.3333333333333" customWidth="1"/>
+    <col min="2" max="2" width="14.2166666666667" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" customWidth="1"/>
+    <col min="4" max="4" width="23.775" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" ht="15" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" ht="15" spans="1:4">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+    <row r="3" ht="15" spans="1:4">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+    <row r="4" ht="15" spans="1:4">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+    <row r="5" ht="15" spans="1:4">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+    <row r="6" ht="15" spans="1:4">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+    <row r="7" ht="15" spans="1:4">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+    <row r="8" ht="15" spans="1:4">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" ht="15" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" ht="15" spans="1:4">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>